<commit_message>
slave marche !!!!! BF cap et avance... tangeant
</commit_message>
<xml_diff>
--- a/correction des gains.xlsx
+++ b/correction des gains.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>tic</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>cap sens trigo</t>
+  </si>
+  <si>
+    <t>ancien gain rot</t>
+  </si>
+  <si>
+    <t>theorique</t>
+  </si>
+  <si>
+    <t>mesuree</t>
+  </si>
+  <si>
+    <t>new gain</t>
   </si>
 </sst>
 </file>
@@ -176,14 +188,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,15 +499,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M14"/>
+  <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
@@ -510,43 +523,43 @@
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -555,7 +568,7 @@
       <c r="C5" s="1">
         <v>1245</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1000</v>
       </c>
       <c r="E5" s="1">
@@ -566,7 +579,7 @@
       <c r="G5" s="1">
         <v>1245</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>1000</v>
       </c>
       <c r="I5" s="1">
@@ -579,13 +592,27 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="C6" s="1">
+        <v>5275</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E6" s="1">
+        <f>D6/C6</f>
+        <v>0.37914691943127959</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="G6" s="1">
+        <v>5301</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I6" s="1">
+        <f>H6/G6</f>
+        <v>0.37728730428221091</v>
+      </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -611,19 +638,19 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="L10" s="5" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="L10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="M10">
@@ -632,29 +659,29 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="4"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -663,7 +690,7 @@
       <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>1000</v>
       </c>
       <c r="E12" s="1">
@@ -674,7 +701,7 @@
       <c r="G12" s="1">
         <v>3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>1000</v>
       </c>
       <c r="I12" s="1">
@@ -704,6 +731,35 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C18">
+        <v>216.56</v>
+      </c>
+      <c r="D18">
+        <v>180</v>
+      </c>
+      <c r="E18">
+        <f>B18*D18/C18</f>
+        <v>4.9870705578130775E-3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
small change, to do -> adoucir la descente et remontee des bras coopr
</commit_message>
<xml_diff>
--- a/correction des gains.xlsx
+++ b/correction des gains.xlsx
@@ -580,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M19"/>
+  <dimension ref="B1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,6 +881,26 @@
       <c r="E19">
         <f>B19*D19/C19</f>
         <v>4.9870705578130775E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4.9870000000000001E-3</v>
+      </c>
+      <c r="C20">
+        <v>324.20999999999998</v>
+      </c>
+      <c r="D20">
+        <v>360</v>
+      </c>
+      <c r="E20">
+        <f>B20*D20/C20</f>
+        <v>5.5375219764967152E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>4.9870000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>